<commit_message>
Adding Excel spreadhseet to play with Visual Builder
</commit_message>
<xml_diff>
--- a/test/OrdersData.xlsx
+++ b/test/OrdersData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cri\Cloud\SpeedToValue\Integration_APIs\TheCastle_projects\GIT_Repos\APIs4SaaSDemo\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0768BAD2-D7FC-4F8E-B443-19B865042E03}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165E97F1-2F75-43CF-9BAB-DCF2747B753F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -1017,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F22" sqref="F22:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1030,7 +1030,7 @@
     <col min="3" max="3" width="20.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1046,8 +1046,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1063,8 +1066,11 @@
       <c r="E2">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1080,8 +1086,11 @@
       <c r="E3">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1097,8 +1106,11 @@
       <c r="E4">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1114,8 +1126,11 @@
       <c r="E5">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1131,8 +1146,11 @@
       <c r="E6">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1148,8 +1166,11 @@
       <c r="E7">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1165,8 +1186,11 @@
       <c r="E8">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1182,8 +1206,11 @@
       <c r="E9">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1199,8 +1226,11 @@
       <c r="E10">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1216,8 +1246,11 @@
       <c r="E11">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1233,8 +1266,11 @@
       <c r="E12">
         <v>17.32</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1250,8 +1286,11 @@
       <c r="E13">
         <v>17.32</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1267,8 +1306,11 @@
       <c r="E14">
         <v>17.32</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1284,8 +1326,11 @@
       <c r="E15">
         <v>17.32</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1301,8 +1346,11 @@
       <c r="E16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1318,8 +1366,11 @@
       <c r="E17">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1335,8 +1386,11 @@
       <c r="E18">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1352,8 +1406,11 @@
       <c r="E19">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1369,8 +1426,11 @@
       <c r="E20">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1386,8 +1446,11 @@
       <c r="E21">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1403,8 +1466,11 @@
       <c r="E22">
         <v>99.99</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1420,8 +1486,11 @@
       <c r="E23">
         <v>99.99</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1437,8 +1506,11 @@
       <c r="E24">
         <v>99.99</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1454,8 +1526,11 @@
       <c r="E25">
         <v>99.99</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1470,6 +1545,9 @@
       </c>
       <c r="E26">
         <v>99.99</v>
+      </c>
+      <c r="F26" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1482,7 +1560,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>